<commit_message>
Erros na lógica de envio de mensagem no whatsapp
vou tirar a parte de abrir e fechar janelas sempre que enviar mensagem para uma pessoa diferente, além de ter que arrumar o loop de busca
</commit_message>
<xml_diff>
--- a/contatos-notificados.xlsx
+++ b/contatos-notificados.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
   <si>
     <t>Mestre</t>
   </si>
@@ -33,6 +33,9 @@
   </si>
   <si>
     <t>contato</t>
+  </si>
+  <si>
+    <t>Pai</t>
   </si>
 </sst>
 </file>
@@ -350,10 +353,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="C4:D5"/>
+  <dimension ref="C4:D6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -378,6 +381,14 @@
         <v>5537998460473</v>
       </c>
     </row>
+    <row r="6" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C6" t="s">
+        <v>3</v>
+      </c>
+      <c r="D6">
+        <v>5537998327615</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Parte de enviar mensagem para contatos OK
Loop de envio de mensagem de whatsapp pronta, estou mexendo no loop de reinicio do sistema  em 300 segundos
</commit_message>
<xml_diff>
--- a/contatos-notificados.xlsx
+++ b/contatos-notificados.xlsx
@@ -42,7 +42,17 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+  <numFmts count="1">
+    <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
+  </numFmts>
+  <fonts count="2" x14ac:knownFonts="1">
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -68,14 +78,18 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="12" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="12" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Vírgula" xfId="1" builtinId="3"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -356,12 +370,12 @@
   <dimension ref="C4:D6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="4" max="4" width="14.42578125" customWidth="1"/>
+    <col min="4" max="4" width="17.42578125" customWidth="1"/>
     <col min="7" max="7" width="23.7109375" customWidth="1"/>
   </cols>
   <sheetData>
@@ -377,7 +391,7 @@
       <c r="C5" t="s">
         <v>0</v>
       </c>
-      <c r="D5">
+      <c r="D5" s="1">
         <v>5537998460473</v>
       </c>
     </row>
@@ -385,7 +399,7 @@
       <c r="C6" t="s">
         <v>3</v>
       </c>
-      <c r="D6">
+      <c r="D6" s="2">
         <v>5537998327615</v>
       </c>
     </row>

</xml_diff>